<commit_message>
pylint on visual code correct
</commit_message>
<xml_diff>
--- a/WppSender/telefones.xlsx
+++ b/WppSender/telefones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VINÍCIUS\Documents\GitHub\MeusProjetos\Wpp-Sender\WppSender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1A156F-7388-4693-BF99-7A0A63E7A541}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617582D1-46C8-4AC7-926D-707CCB036018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>nome_proprietario</t>
   </si>
@@ -28,19 +28,58 @@
     <t>WppSender</t>
   </si>
   <si>
-    <t>Vinicius</t>
-  </si>
-  <si>
-    <t>guilherme</t>
-  </si>
-  <si>
-    <t>maria</t>
-  </si>
-  <si>
-    <t>ester</t>
-  </si>
-  <si>
-    <t>tiA</t>
+    <t>Ana Carolina</t>
+  </si>
+  <si>
+    <t>Anna Lena</t>
+  </si>
+  <si>
+    <t>Jhonatan</t>
+  </si>
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>Brenda</t>
+  </si>
+  <si>
+    <t>Caeh</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>Juliana</t>
+  </si>
+  <si>
+    <t>Larissa</t>
+  </si>
+  <si>
+    <t>5532984884745</t>
+  </si>
+  <si>
+    <t>5532988191429</t>
+  </si>
+  <si>
+    <t>5532988923958</t>
+  </si>
+  <si>
+    <t>5532984427134</t>
+  </si>
+  <si>
+    <t>5532988213508</t>
+  </si>
+  <si>
+    <t>5532991418096</t>
+  </si>
+  <si>
+    <t>5532984700198</t>
+  </si>
+  <si>
+    <t>5532988858637</t>
+  </si>
+  <si>
+    <t>5532999798051</t>
   </si>
 </sst>
 </file>
@@ -882,16 +921,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C2" sqref="C2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -906,48 +946,72 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
-        <v>5521987471901</v>
+      <c r="B2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
-        <v>5521987471901</v>
+      <c r="B3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
-        <v>5521987471901</v>
+      <c r="B4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>5521987471901</v>
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>5521987471901</v>
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>5521987471901</v>
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>